<commit_message>
Updated 1945, 1946 and 1948
</commit_message>
<xml_diff>
--- a/Seasons/Football History.xlsx
+++ b/Seasons/Football History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugs&amp;Fred\Documents\Fred\ROSM\Website\public_html\Seasons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD695F4-B645-42B2-BC42-432C39DCAAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F5B623-1C0C-40C7-95C6-87F424F5B009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8C7F2BF-BA1F-4802-BC8C-4DC7AFA8B3A8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="407">
   <si>
     <t>Opponent</t>
   </si>
@@ -1674,34 +1674,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> was named to the All-SOC (South Oakland County) Football team.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Al Chevalier and Ed Casey (Class of '49) served as the head coach. Coach Chevalier, a former Pro Canadian Football player, had high expectations with the 13 returning letterman. After 3 games Al Chevalier resigns, stating the time and travel as the factors (he was commuting daily from Windsor). He had become the first coach on the faculty of St. Mary's and left with the shortest tenure. Ed Casey, a star player from the 1948 2nd Division Co-Champs, was installed as the interim coach. Casey was to be inducted into the Navy in December of 1952. He later returned as the Irish head coach in 1957. The team finishes with a 3-3-1 record. While the defense was solid in all but one game, the offense never got untracked scoring only 45 points all season. A season highlight was upsetting rival St. James in the season finale 12-6.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dick Parker</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> was named to the All-SOC (South Oakland County) Football team.
-</t>
     </r>
   </si>
   <si>
@@ -3445,6 +3417,55 @@
         <scheme val="minor"/>
       </rPr>
       <t>was named to the Detroit News Class D All-State Team.</t>
+    </r>
+  </si>
+  <si>
+    <t>1961 Final Record</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Al Chevalier and Ed Casey (Class of '49) served as the head coach.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Coach Chevalier, a former Pro Canadian Football player, had high expectations with the 13 returning letterman. After 3 games Al Chevalier resigns, stating the time and travel as the factors (he was commuting daily from Windsor). He had become the first coach on the faculty of St. Mary's and left with the shortest tenure. Ed Casey, a star player from the 1948 2nd Division Co-Champs, was installed as the interim coach. Casey was to be inducted into the Navy in December of 1952. He later returned as the Irish head coach in 1957. The team finishes with a 3-3-1 record. While the defense was solid in all but one game, the offense never got untracked scoring only 45 points all season. A season highlight was upsetting rival St. James in the season finale 12-6.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dick Parker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> was named to the All-SOC (South Oakland County) Football team.
+</t>
     </r>
   </si>
 </sst>
@@ -3916,7 +3937,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3927,7 +3948,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3935,6 +3959,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3945,29 +3984,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3975,11 +3996,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6628,8 +6649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2FFFC7-E182-47AD-9B1B-521106FC03D6}">
   <dimension ref="A1:G2039"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A475" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G483" sqref="G483:G491"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G266" sqref="G266:G274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6656,17 +6677,17 @@
         <v>183</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="60" t="s">
         <v>182</v>
       </c>
       <c r="B2" s="2">
@@ -6684,12 +6705,12 @@
       <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="57" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="2">
         <v>10152</v>
       </c>
@@ -6705,10 +6726,10 @@
       <c r="F3" s="7">
         <v>12</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="2">
         <v>10156</v>
       </c>
@@ -6724,10 +6745,10 @@
       <c r="F4" s="7">
         <v>14</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="2">
         <v>10171</v>
       </c>
@@ -6743,37 +6764,37 @@
       <c r="F5" s="7">
         <v>23</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="52"/>
+      <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="2"/>
       <c r="C9" s="12" t="s">
         <v>45</v>
@@ -6789,7 +6810,7 @@
         <f>SUM(F2:F8)</f>
         <v>49</v>
       </c>
-      <c r="G9" s="53"/>
+      <c r="G9" s="54"/>
     </row>
     <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
@@ -6805,17 +6826,17 @@
         <v>183</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="60" t="s">
         <v>184</v>
       </c>
       <c r="B11" s="2">
@@ -6833,12 +6854,12 @@
       <c r="F11" s="7">
         <v>0</v>
       </c>
-      <c r="G11" s="51" t="s">
-        <v>389</v>
+      <c r="G11" s="57" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="2">
         <v>10506</v>
       </c>
@@ -6854,10 +6875,10 @@
       <c r="F12" s="7">
         <v>32</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="2">
         <v>10513</v>
       </c>
@@ -6873,10 +6894,10 @@
       <c r="F13" s="7">
         <v>20</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="53"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="2">
         <v>10527</v>
       </c>
@@ -6892,10 +6913,10 @@
       <c r="F14" s="7">
         <v>19</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="2">
         <v>10541</v>
       </c>
@@ -6911,10 +6932,10 @@
       <c r="F15" s="7">
         <v>45</v>
       </c>
-      <c r="G15" s="52"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="2">
         <v>10548</v>
       </c>
@@ -6930,10 +6951,10 @@
       <c r="F16" s="7">
         <v>7</v>
       </c>
-      <c r="G16" s="52"/>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="2">
         <v>10555</v>
       </c>
@@ -6949,10 +6970,10 @@
       <c r="F17" s="7">
         <v>0</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="2">
         <v>10561</v>
       </c>
@@ -6968,10 +6989,10 @@
       <c r="F18" s="7">
         <v>6</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="2"/>
       <c r="C19" s="16" t="s">
         <v>46</v>
@@ -6987,7 +7008,7 @@
         <f>SUM(F11:F18)</f>
         <v>129</v>
       </c>
-      <c r="G19" s="53"/>
+      <c r="G19" s="54"/>
     </row>
     <row r="20" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
@@ -7003,17 +7024,17 @@
         <v>183</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="61" t="s">
         <v>185</v>
       </c>
       <c r="B21" s="2">
@@ -7031,12 +7052,12 @@
       <c r="F21" s="7">
         <v>27</v>
       </c>
-      <c r="G21" s="51" t="s">
+      <c r="G21" s="57" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="2">
         <v>10870</v>
       </c>
@@ -7052,10 +7073,10 @@
       <c r="F22" s="7">
         <v>13</v>
       </c>
-      <c r="G22" s="52"/>
+      <c r="G22" s="53"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="2">
         <v>10877</v>
       </c>
@@ -7071,10 +7092,10 @@
       <c r="F23" s="7">
         <v>13</v>
       </c>
-      <c r="G23" s="52"/>
+      <c r="G23" s="53"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="2">
         <v>10884</v>
       </c>
@@ -7090,10 +7111,10 @@
       <c r="F24" s="7">
         <v>18</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="53"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="2">
         <v>10891</v>
       </c>
@@ -7109,10 +7130,10 @@
       <c r="F25" s="7">
         <v>24</v>
       </c>
-      <c r="G25" s="52"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="2">
         <v>10898</v>
       </c>
@@ -7128,10 +7149,10 @@
       <c r="F26" s="7">
         <v>7</v>
       </c>
-      <c r="G26" s="52"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="2">
         <v>10905</v>
       </c>
@@ -7147,10 +7168,10 @@
       <c r="F27" s="7">
         <v>0</v>
       </c>
-      <c r="G27" s="52"/>
+      <c r="G27" s="53"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="2">
         <v>10912</v>
       </c>
@@ -7166,10 +7187,10 @@
       <c r="F28" s="7">
         <v>0</v>
       </c>
-      <c r="G28" s="52"/>
+      <c r="G28" s="53"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="2" t="s">
         <v>78</v>
       </c>
@@ -7185,10 +7206,10 @@
       <c r="F29" s="7">
         <v>0</v>
       </c>
-      <c r="G29" s="52"/>
+      <c r="G29" s="53"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="2">
         <v>10917</v>
       </c>
@@ -7204,10 +7225,10 @@
       <c r="F30" s="7">
         <v>0</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="53"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="2">
         <v>10925</v>
       </c>
@@ -7223,10 +7244,10 @@
       <c r="F31" s="7">
         <v>7</v>
       </c>
-      <c r="G31" s="52"/>
+      <c r="G31" s="53"/>
     </row>
     <row r="32" spans="1:7" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16" t="s">
         <v>47</v>
@@ -7242,7 +7263,7 @@
         <f>SUM(F21:F31)</f>
         <v>109</v>
       </c>
-      <c r="G32" s="53"/>
+      <c r="G32" s="54"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
@@ -7258,10 +7279,10 @@
         <v>183</v>
       </c>
       <c r="E33" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F33" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>9</v>
@@ -7286,7 +7307,7 @@
       <c r="F34" s="7">
         <v>0</v>
       </c>
-      <c r="G34" s="51" t="s">
+      <c r="G34" s="57" t="s">
         <v>337</v>
       </c>
     </row>
@@ -7307,7 +7328,7 @@
       <c r="F35" s="7">
         <v>0</v>
       </c>
-      <c r="G35" s="52"/>
+      <c r="G35" s="53"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="45"/>
@@ -7326,7 +7347,7 @@
       <c r="F36" s="7">
         <v>0</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="53"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
@@ -7345,7 +7366,7 @@
       <c r="F37" s="7">
         <v>0</v>
       </c>
-      <c r="G37" s="52"/>
+      <c r="G37" s="53"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="45"/>
@@ -7364,7 +7385,7 @@
       <c r="F38" s="7">
         <v>6</v>
       </c>
-      <c r="G38" s="52"/>
+      <c r="G38" s="53"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
@@ -7383,7 +7404,7 @@
       <c r="F39" s="7">
         <v>0</v>
       </c>
-      <c r="G39" s="52"/>
+      <c r="G39" s="53"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="45"/>
@@ -7402,7 +7423,7 @@
       <c r="F40" s="7">
         <v>0</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="53"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="45"/>
@@ -7421,7 +7442,7 @@
       <c r="F41" s="7">
         <v>0</v>
       </c>
-      <c r="G41" s="52"/>
+      <c r="G41" s="53"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="45"/>
@@ -7440,7 +7461,7 @@
       <c r="F42" s="7">
         <v>0</v>
       </c>
-      <c r="G42" s="52"/>
+      <c r="G42" s="53"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="46"/>
@@ -7459,7 +7480,7 @@
         <f>SUM(F34:F42)</f>
         <v>6</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="54"/>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
@@ -7475,17 +7496,17 @@
         <v>183</v>
       </c>
       <c r="E44" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F44" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47" t="s">
+      <c r="A45" s="59" t="s">
         <v>187</v>
       </c>
       <c r="B45" s="2">
@@ -7504,7 +7525,7 @@
         <v>7</v>
       </c>
       <c r="G45" s="50" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -7551,7 +7572,7 @@
         <v>11619</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>1</v>
@@ -7666,7 +7687,7 @@
         <v>49</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E54" s="22">
         <f>SUM(E45:E53)</f>
@@ -7692,10 +7713,10 @@
         <v>183</v>
       </c>
       <c r="E55" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F55" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F55" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>9</v>
@@ -7890,10 +7911,10 @@
         <v>183</v>
       </c>
       <c r="E65" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F65" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F65" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G65" s="9" t="s">
         <v>9</v>
@@ -7919,7 +7940,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="50" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -8101,17 +8122,17 @@
         <v>183</v>
       </c>
       <c r="E76" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F76" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F76" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G76" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="58" t="s">
+      <c r="A77" s="55" t="s">
         <v>190</v>
       </c>
       <c r="B77" s="2">
@@ -8129,12 +8150,12 @@
       <c r="F77" s="7">
         <v>6</v>
       </c>
-      <c r="G77" s="51" t="s">
-        <v>399</v>
+      <c r="G77" s="57" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="57"/>
+      <c r="A78" s="56"/>
       <c r="B78" s="2">
         <v>12699</v>
       </c>
@@ -8150,10 +8171,10 @@
       <c r="F78" s="7">
         <v>12</v>
       </c>
-      <c r="G78" s="52"/>
+      <c r="G78" s="53"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="57"/>
+      <c r="A79" s="56"/>
       <c r="B79" s="2">
         <v>12705</v>
       </c>
@@ -8169,10 +8190,10 @@
       <c r="F79" s="7">
         <v>15</v>
       </c>
-      <c r="G79" s="52"/>
+      <c r="G79" s="53"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="57"/>
+      <c r="A80" s="56"/>
       <c r="B80" s="2">
         <v>12713</v>
       </c>
@@ -8188,10 +8209,10 @@
       <c r="F80" s="7">
         <v>0</v>
       </c>
-      <c r="G80" s="52"/>
+      <c r="G80" s="53"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="57"/>
+      <c r="A81" s="56"/>
       <c r="B81" s="2">
         <v>12720</v>
       </c>
@@ -8207,10 +8228,10 @@
       <c r="F81" s="7">
         <v>0</v>
       </c>
-      <c r="G81" s="52"/>
+      <c r="G81" s="53"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="57"/>
+      <c r="A82" s="56"/>
       <c r="B82" s="2">
         <v>12727</v>
       </c>
@@ -8226,10 +8247,10 @@
       <c r="F82" s="7">
         <v>0</v>
       </c>
-      <c r="G82" s="52"/>
+      <c r="G82" s="53"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="57"/>
+      <c r="A83" s="56"/>
       <c r="B83" s="40">
         <v>12734</v>
       </c>
@@ -8245,10 +8266,10 @@
       <c r="F83" s="43">
         <v>0</v>
       </c>
-      <c r="G83" s="52"/>
+      <c r="G83" s="53"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="57"/>
+      <c r="A84" s="56"/>
       <c r="B84" s="2">
         <v>12741</v>
       </c>
@@ -8264,35 +8285,35 @@
       <c r="F84" s="7">
         <v>0</v>
       </c>
-      <c r="G84" s="52"/>
+      <c r="G84" s="53"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="57"/>
+      <c r="A85" s="56"/>
       <c r="B85" s="2"/>
       <c r="D85" s="3"/>
       <c r="E85" s="6"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="52"/>
+      <c r="G85" s="53"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="57"/>
+      <c r="A86" s="56"/>
       <c r="B86" s="2"/>
       <c r="D86" s="3"/>
       <c r="E86" s="6"/>
       <c r="F86" s="7"/>
-      <c r="G86" s="52"/>
+      <c r="G86" s="53"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="57"/>
+      <c r="A87" s="56"/>
       <c r="B87" s="3"/>
       <c r="C87" s="20"/>
       <c r="D87" s="21"/>
       <c r="E87" s="22"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="52"/>
+      <c r="G87" s="53"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="57"/>
+      <c r="A88" s="56"/>
       <c r="B88" s="35"/>
       <c r="C88" s="39" t="s">
         <v>339</v>
@@ -8300,10 +8321,10 @@
       <c r="D88" s="36"/>
       <c r="E88" s="37"/>
       <c r="F88" s="38"/>
-      <c r="G88" s="52"/>
+      <c r="G88" s="53"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="57"/>
+      <c r="A89" s="56"/>
       <c r="B89" s="35"/>
       <c r="C89" s="20" t="s">
         <v>43</v>
@@ -8319,7 +8340,7 @@
         <f>SUM(F77:F88)</f>
         <v>33</v>
       </c>
-      <c r="G89" s="53"/>
+      <c r="G89" s="54"/>
     </row>
     <row r="90" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
@@ -8335,17 +8356,17 @@
         <v>183</v>
       </c>
       <c r="E90" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F90" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F90" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G90" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="57" t="s">
+      <c r="A91" s="56" t="s">
         <v>191</v>
       </c>
       <c r="B91" s="2">
@@ -8364,11 +8385,11 @@
         <v>0</v>
       </c>
       <c r="G91" s="50" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="57"/>
+      <c r="A92" s="56"/>
       <c r="B92" s="2">
         <v>13069</v>
       </c>
@@ -8387,7 +8408,7 @@
       <c r="G92" s="50"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="57"/>
+      <c r="A93" s="56"/>
       <c r="B93" s="2">
         <v>13077</v>
       </c>
@@ -8406,7 +8427,7 @@
       <c r="G93" s="50"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="57"/>
+      <c r="A94" s="56"/>
       <c r="B94" s="2">
         <v>13084</v>
       </c>
@@ -8425,7 +8446,7 @@
       <c r="G94" s="50"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="57"/>
+      <c r="A95" s="56"/>
       <c r="B95" s="2">
         <v>13091</v>
       </c>
@@ -8444,7 +8465,7 @@
       <c r="G95" s="50"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="57"/>
+      <c r="A96" s="56"/>
       <c r="B96" s="2">
         <v>13098</v>
       </c>
@@ -8463,7 +8484,7 @@
       <c r="G96" s="50"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="57"/>
+      <c r="A97" s="56"/>
       <c r="B97" s="2">
         <v>13105</v>
       </c>
@@ -8482,7 +8503,7 @@
       <c r="G97" s="50"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="57"/>
+      <c r="A98" s="56"/>
       <c r="B98" s="2">
         <v>13112</v>
       </c>
@@ -8501,7 +8522,7 @@
       <c r="G98" s="50"/>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="57"/>
+      <c r="A99" s="56"/>
       <c r="B99" s="3"/>
       <c r="C99" s="20" t="s">
         <v>44</v>
@@ -8533,10 +8554,10 @@
         <v>183</v>
       </c>
       <c r="E100" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F100" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F100" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G100" s="9" t="s">
         <v>9</v>
@@ -8731,10 +8752,10 @@
         <v>183</v>
       </c>
       <c r="E110" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F110" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F110" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G110" s="9" t="s">
         <v>9</v>
@@ -8929,10 +8950,10 @@
         <v>183</v>
       </c>
       <c r="E120" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F120" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F120" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>9</v>
@@ -9127,10 +9148,10 @@
         <v>183</v>
       </c>
       <c r="E130" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F130" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F130" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G130" s="9" t="s">
         <v>69</v>
@@ -9319,10 +9340,10 @@
         <v>183</v>
       </c>
       <c r="E140" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F140" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F140" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G140" s="9" t="s">
         <v>9</v>
@@ -9498,10 +9519,10 @@
         <v>183</v>
       </c>
       <c r="E149" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F149" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F149" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G149" s="9" t="s">
         <v>9</v>
@@ -9526,7 +9547,7 @@
       <c r="F150" s="7">
         <v>12</v>
       </c>
-      <c r="G150" s="61" t="s">
+      <c r="G150" s="52" t="s">
         <v>346</v>
       </c>
     </row>
@@ -9547,7 +9568,7 @@
       <c r="F151" s="7">
         <v>0</v>
       </c>
-      <c r="G151" s="52"/>
+      <c r="G151" s="53"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="45"/>
@@ -9566,7 +9587,7 @@
       <c r="F152" s="7">
         <v>13</v>
       </c>
-      <c r="G152" s="52"/>
+      <c r="G152" s="53"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="45"/>
@@ -9585,7 +9606,7 @@
       <c r="F153" s="7">
         <v>0</v>
       </c>
-      <c r="G153" s="52"/>
+      <c r="G153" s="53"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="45"/>
@@ -9604,7 +9625,7 @@
       <c r="F154" s="7">
         <v>31</v>
       </c>
-      <c r="G154" s="52"/>
+      <c r="G154" s="53"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="45"/>
@@ -9623,7 +9644,7 @@
       <c r="F155" s="7">
         <v>13</v>
       </c>
-      <c r="G155" s="52"/>
+      <c r="G155" s="53"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="45"/>
@@ -9642,7 +9663,7 @@
       <c r="F156" s="7">
         <v>21</v>
       </c>
-      <c r="G156" s="52"/>
+      <c r="G156" s="53"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="45"/>
@@ -9661,7 +9682,7 @@
       <c r="F157" s="7">
         <v>38</v>
       </c>
-      <c r="G157" s="52"/>
+      <c r="G157" s="53"/>
     </row>
     <row r="158" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="46"/>
@@ -9680,7 +9701,7 @@
         <f>SUM(F150:F157)</f>
         <v>128</v>
       </c>
-      <c r="G158" s="53"/>
+      <c r="G158" s="54"/>
     </row>
     <row r="159" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="28" t="s">
@@ -9696,10 +9717,10 @@
         <v>183</v>
       </c>
       <c r="E159" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F159" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F159" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G159" s="9" t="s">
         <v>9</v>
@@ -9724,7 +9745,7 @@
       <c r="F160" s="5">
         <v>7</v>
       </c>
-      <c r="G160" s="60" t="s">
+      <c r="G160" s="51" t="s">
         <v>347</v>
       </c>
     </row>
@@ -9888,10 +9909,10 @@
         <v>183</v>
       </c>
       <c r="E169" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F169" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F169" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G169" s="9" t="s">
         <v>9</v>
@@ -9916,8 +9937,8 @@
       <c r="F170" s="5">
         <v>12</v>
       </c>
-      <c r="G170" s="60" t="s">
-        <v>390</v>
+      <c r="G170" s="51" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -10086,10 +10107,10 @@
         <v>183</v>
       </c>
       <c r="E179" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F179" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F179" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G179" s="9" t="s">
         <v>9</v>
@@ -10284,10 +10305,10 @@
         <v>183</v>
       </c>
       <c r="E189" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F189" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F189" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G189" s="9" t="s">
         <v>9</v>
@@ -10312,7 +10333,7 @@
       <c r="F190" s="5">
         <v>26</v>
       </c>
-      <c r="G190" s="60" t="s">
+      <c r="G190" s="51" t="s">
         <v>349</v>
       </c>
     </row>
@@ -10482,17 +10503,17 @@
         <v>183</v>
       </c>
       <c r="E199" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F199" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F199" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G199" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A200" s="47" t="s">
+      <c r="A200" s="59" t="s">
         <v>202</v>
       </c>
       <c r="B200" s="2">
@@ -10510,8 +10531,8 @@
       <c r="F200" s="5">
         <v>7</v>
       </c>
-      <c r="G200" s="59" t="s">
-        <v>396</v>
+      <c r="G200" s="58" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -10664,7 +10685,7 @@
       <c r="F208" s="5">
         <v>7</v>
       </c>
-      <c r="G208" s="51"/>
+      <c r="G208" s="57"/>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="48"/>
@@ -10673,7 +10694,7 @@
       <c r="D209" s="3"/>
       <c r="E209" s="8"/>
       <c r="F209" s="5"/>
-      <c r="G209" s="51"/>
+      <c r="G209" s="57"/>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="48"/>
@@ -10682,7 +10703,7 @@
       <c r="D210" s="3"/>
       <c r="E210" s="8"/>
       <c r="F210" s="5"/>
-      <c r="G210" s="51"/>
+      <c r="G210" s="57"/>
     </row>
     <row r="211" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="49"/>
@@ -10701,7 +10722,7 @@
         <f>SUM(F200:F208)</f>
         <v>16</v>
       </c>
-      <c r="G211" s="51"/>
+      <c r="G211" s="57"/>
     </row>
     <row r="212" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="28" t="s">
@@ -10717,10 +10738,10 @@
         <v>183</v>
       </c>
       <c r="E212" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F212" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F212" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G212" s="9" t="s">
         <v>9</v>
@@ -10745,7 +10766,7 @@
       <c r="F213" s="7">
         <v>13</v>
       </c>
-      <c r="G213" s="60" t="s">
+      <c r="G213" s="51" t="s">
         <v>351</v>
       </c>
     </row>
@@ -10934,17 +10955,17 @@
         <v>183</v>
       </c>
       <c r="E223" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F223" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F223" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G223" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224" s="58" t="s">
+      <c r="A224" s="55" t="s">
         <v>204</v>
       </c>
       <c r="B224" s="2">
@@ -10967,7 +10988,7 @@
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225" s="57"/>
+      <c r="A225" s="56"/>
       <c r="B225" s="2">
         <v>17802</v>
       </c>
@@ -10986,7 +11007,7 @@
       <c r="G225" s="50"/>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" s="57"/>
+      <c r="A226" s="56"/>
       <c r="B226" s="4">
         <v>17809</v>
       </c>
@@ -11005,7 +11026,7 @@
       <c r="G226" s="50"/>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A227" s="57"/>
+      <c r="A227" s="56"/>
       <c r="B227" s="2">
         <v>17814</v>
       </c>
@@ -11024,7 +11045,7 @@
       <c r="G227" s="50"/>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A228" s="57"/>
+      <c r="A228" s="56"/>
       <c r="B228" s="2">
         <v>17822</v>
       </c>
@@ -11043,7 +11064,7 @@
       <c r="G228" s="50"/>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A229" s="57"/>
+      <c r="A229" s="56"/>
       <c r="B229" s="2">
         <v>17830</v>
       </c>
@@ -11062,7 +11083,7 @@
       <c r="G229" s="50"/>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="57"/>
+      <c r="A230" s="56"/>
       <c r="B230" s="2">
         <v>17844</v>
       </c>
@@ -11081,7 +11102,7 @@
       <c r="G230" s="50"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="57"/>
+      <c r="A231" s="56"/>
       <c r="B231" s="4">
         <v>17852</v>
       </c>
@@ -11100,7 +11121,7 @@
       <c r="G231" s="50"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A232" s="57"/>
+      <c r="A232" s="56"/>
       <c r="B232" s="4"/>
       <c r="C232" s="3"/>
       <c r="D232" s="3"/>
@@ -11109,7 +11130,7 @@
       <c r="G232" s="50"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A233" s="57"/>
+      <c r="A233" s="56"/>
       <c r="B233" s="4"/>
       <c r="C233" s="3"/>
       <c r="D233" s="3"/>
@@ -11118,7 +11139,7 @@
       <c r="G233" s="50"/>
     </row>
     <row r="234" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="57"/>
+      <c r="A234" s="56"/>
       <c r="B234" s="3"/>
       <c r="C234" s="20" t="s">
         <v>139</v>
@@ -11150,10 +11171,10 @@
         <v>183</v>
       </c>
       <c r="E235" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F235" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F235" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G235" s="9" t="s">
         <v>9</v>
@@ -11332,7 +11353,7 @@
         <f>SUM(F236:F243)</f>
         <v>82</v>
       </c>
-      <c r="G244" s="51"/>
+      <c r="G244" s="57"/>
     </row>
     <row r="245" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="28" t="s">
@@ -11348,10 +11369,10 @@
         <v>183</v>
       </c>
       <c r="E245" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F245" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F245" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G245" s="9" t="s">
         <v>9</v>
@@ -11376,7 +11397,7 @@
       <c r="F246" s="5">
         <v>31</v>
       </c>
-      <c r="G246" s="60" t="s">
+      <c r="G246" s="51" t="s">
         <v>356</v>
       </c>
     </row>
@@ -11546,10 +11567,10 @@
         <v>183</v>
       </c>
       <c r="E255" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F255" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F255" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G255" s="9" t="s">
         <v>9</v>
@@ -11744,10 +11765,10 @@
         <v>183</v>
       </c>
       <c r="E265" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F265" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F265" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G265" s="9" t="s">
         <v>9</v>
@@ -11773,7 +11794,7 @@
         <v>6</v>
       </c>
       <c r="G266" s="50" t="s">
-        <v>358</v>
+        <v>406</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -11926,7 +11947,7 @@
     </row>
     <row r="275" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B275" s="9">
         <v>1953</v>
@@ -11938,10 +11959,10 @@
         <v>183</v>
       </c>
       <c r="E275" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F275" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F275" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G275" s="9" t="s">
         <v>9</v>
@@ -11967,7 +11988,7 @@
         <v>0</v>
       </c>
       <c r="G276" s="50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
@@ -12105,7 +12126,7 @@
     </row>
     <row r="284" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B284" s="9">
         <v>1954</v>
@@ -12117,10 +12138,10 @@
         <v>183</v>
       </c>
       <c r="E284" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F284" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F284" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G284" s="9" t="s">
         <v>9</v>
@@ -12145,8 +12166,8 @@
       <c r="F285" s="7">
         <v>19</v>
       </c>
-      <c r="G285" s="60" t="s">
-        <v>361</v>
+      <c r="G285" s="51" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
@@ -12315,10 +12336,10 @@
         <v>183</v>
       </c>
       <c r="E294" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F294" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F294" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G294" s="9" t="s">
         <v>9</v>
@@ -12344,7 +12365,7 @@
         <v>12</v>
       </c>
       <c r="G295" s="50" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
@@ -12513,10 +12534,10 @@
         <v>183</v>
       </c>
       <c r="E304" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F304" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F304" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G304" s="9" t="s">
         <v>9</v>
@@ -12541,8 +12562,8 @@
       <c r="F305" s="5">
         <v>12</v>
       </c>
-      <c r="G305" s="60" t="s">
-        <v>363</v>
+      <c r="G305" s="51" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
@@ -12711,10 +12732,10 @@
         <v>183</v>
       </c>
       <c r="E314" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F314" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F314" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G314" s="9" t="s">
         <v>9</v>
@@ -12740,7 +12761,7 @@
         <v>7</v>
       </c>
       <c r="G315" s="50" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.25">
@@ -12908,7 +12929,7 @@
     </row>
     <row r="325" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B325" s="9">
         <v>1958</v>
@@ -12920,10 +12941,10 @@
         <v>183</v>
       </c>
       <c r="E325" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F325" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F325" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G325" s="9" t="s">
         <v>9</v>
@@ -12949,7 +12970,7 @@
         <v>18</v>
       </c>
       <c r="G326" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.25">
@@ -13106,7 +13127,7 @@
     </row>
     <row r="335" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B335" s="9">
         <v>1959</v>
@@ -13118,10 +13139,10 @@
         <v>183</v>
       </c>
       <c r="E335" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F335" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F335" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G335" s="9" t="s">
         <v>9</v>
@@ -13147,7 +13168,7 @@
         <v>20</v>
       </c>
       <c r="G336" s="50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.25">
@@ -13316,10 +13337,10 @@
         <v>183</v>
       </c>
       <c r="E345" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F345" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F345" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G345" s="9" t="s">
         <v>9</v>
@@ -13345,7 +13366,7 @@
         <v>19</v>
       </c>
       <c r="G346" s="50" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.25">
@@ -13514,10 +13535,10 @@
         <v>183</v>
       </c>
       <c r="E355" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F355" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F355" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G355" s="9" t="s">
         <v>9</v>
@@ -13543,7 +13564,7 @@
         <v>6</v>
       </c>
       <c r="G356" s="50" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
@@ -13683,7 +13704,7 @@
       <c r="A364" s="46"/>
       <c r="B364" s="3"/>
       <c r="C364" s="20" t="s">
-        <v>152</v>
+        <v>405</v>
       </c>
       <c r="D364" s="21" t="s">
         <v>75</v>
@@ -13712,10 +13733,10 @@
         <v>183</v>
       </c>
       <c r="E365" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F365" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F365" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G365" s="9" t="s">
         <v>9</v>
@@ -13741,7 +13762,7 @@
         <v>7</v>
       </c>
       <c r="G366" s="50" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
@@ -13750,7 +13771,7 @@
         <v>22919</v>
       </c>
       <c r="C367" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D367" s="3" t="s">
         <v>5</v>
@@ -13891,10 +13912,10 @@
         <v>183</v>
       </c>
       <c r="E374" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F374" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F374" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G374" s="9" t="s">
         <v>9</v>
@@ -13920,7 +13941,7 @@
         <v>20</v>
       </c>
       <c r="G375" s="50" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
@@ -13948,7 +13969,7 @@
         <v>23283</v>
       </c>
       <c r="C377" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D377" s="3" t="s">
         <v>1</v>
@@ -14070,10 +14091,10 @@
         <v>183</v>
       </c>
       <c r="E383" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F383" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F383" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G383" s="9" t="s">
         <v>9</v>
@@ -14087,7 +14108,7 @@
         <v>23640</v>
       </c>
       <c r="C384" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D384" s="3" t="s">
         <v>4</v>
@@ -14099,7 +14120,7 @@
         <v>0</v>
       </c>
       <c r="G384" s="50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.25">
@@ -14249,10 +14270,10 @@
         <v>183</v>
       </c>
       <c r="E392" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F392" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F392" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G392" s="9" t="s">
         <v>9</v>
@@ -14278,7 +14299,7 @@
         <v>6</v>
       </c>
       <c r="G393" s="50" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
@@ -14428,10 +14449,10 @@
         <v>183</v>
       </c>
       <c r="E401" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F401" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F401" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G401" s="9" t="s">
         <v>9</v>
@@ -14457,7 +14478,7 @@
         <v>19</v>
       </c>
       <c r="G402" s="50" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
@@ -14607,10 +14628,10 @@
         <v>183</v>
       </c>
       <c r="E410" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F410" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F410" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G410" s="9" t="s">
         <v>9</v>
@@ -14636,7 +14657,7 @@
         <v>6</v>
       </c>
       <c r="G411" s="50" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.25">
@@ -14805,10 +14826,10 @@
         <v>183</v>
       </c>
       <c r="E420" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F420" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F420" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G420" s="9" t="s">
         <v>9</v>
@@ -14834,7 +14855,7 @@
         <v>14</v>
       </c>
       <c r="G421" s="50" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.25">
@@ -15003,10 +15024,10 @@
         <v>183</v>
       </c>
       <c r="E430" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F430" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F430" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G430" s="9" t="s">
         <v>9</v>
@@ -15032,7 +15053,7 @@
         <v>38</v>
       </c>
       <c r="G431" s="50" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="432" spans="1:7" x14ac:dyDescent="0.25">
@@ -15219,10 +15240,10 @@
         <v>183</v>
       </c>
       <c r="E442" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F442" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F442" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G442" s="9" t="s">
         <v>9</v>
@@ -15248,7 +15269,7 @@
         <v>6</v>
       </c>
       <c r="G443" s="50" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="444" spans="1:7" x14ac:dyDescent="0.25">
@@ -15417,10 +15438,10 @@
         <v>183</v>
       </c>
       <c r="E452" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F452" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F452" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G452" s="9" t="s">
         <v>179</v>
@@ -15446,7 +15467,7 @@
         <v>0</v>
       </c>
       <c r="G453" s="50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.25">
@@ -15615,10 +15636,10 @@
         <v>183</v>
       </c>
       <c r="E462" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F462" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F462" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G462" s="9" t="s">
         <v>9</v>
@@ -15644,7 +15665,7 @@
         <v>28</v>
       </c>
       <c r="G463" s="50" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
@@ -15813,10 +15834,10 @@
         <v>183</v>
       </c>
       <c r="E472" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F472" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F472" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G472" s="9" t="s">
         <v>9</v>
@@ -15841,8 +15862,8 @@
       <c r="F473" s="5">
         <v>19</v>
       </c>
-      <c r="G473" s="60" t="s">
-        <v>380</v>
+      <c r="G473" s="51" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.25">
@@ -16011,10 +16032,10 @@
         <v>183</v>
       </c>
       <c r="E482" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F482" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F482" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G482" s="9" t="s">
         <v>9</v>
@@ -16040,7 +16061,7 @@
         <v>6</v>
       </c>
       <c r="G483" s="50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="484" spans="1:7" x14ac:dyDescent="0.25">
@@ -16209,10 +16230,10 @@
         <v>183</v>
       </c>
       <c r="E492" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F492" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F492" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G492" s="9" t="s">
         <v>9</v>
@@ -16238,7 +16259,7 @@
         <v>6</v>
       </c>
       <c r="G493" s="50" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
@@ -16407,17 +16428,17 @@
         <v>183</v>
       </c>
       <c r="E502" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F502" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F502" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G502" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A503" s="62" t="s">
+      <c r="A503" s="47" t="s">
         <v>232</v>
       </c>
       <c r="B503" s="2">
@@ -16436,7 +16457,7 @@
         <v>0</v>
       </c>
       <c r="G503" s="50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
@@ -16669,10 +16690,10 @@
         <v>183</v>
       </c>
       <c r="E518" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F518" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F518" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G518" s="9" t="s">
         <v>9</v>
@@ -16698,7 +16719,7 @@
         <v>12</v>
       </c>
       <c r="G519" s="50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="520" spans="1:7" x14ac:dyDescent="0.25">
@@ -16886,10 +16907,10 @@
         <v>183</v>
       </c>
       <c r="E529" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F529" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F529" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G529" s="9" t="s">
         <v>9</v>
@@ -16915,7 +16936,7 @@
         <v>40</v>
       </c>
       <c r="G530" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="531" spans="1:7" x14ac:dyDescent="0.25">
@@ -17084,10 +17105,10 @@
         <v>183</v>
       </c>
       <c r="E539" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F539" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F539" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G539" s="9" t="s">
         <v>9</v>
@@ -17113,7 +17134,7 @@
         <v>16</v>
       </c>
       <c r="G540" s="50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
@@ -17301,10 +17322,10 @@
         <v>183</v>
       </c>
       <c r="E550" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F550" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F550" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G550" s="9" t="s">
         <v>9</v>
@@ -17330,7 +17351,7 @@
         <v>39</v>
       </c>
       <c r="G551" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="552" spans="1:7" x14ac:dyDescent="0.25">
@@ -17518,10 +17539,10 @@
         <v>183</v>
       </c>
       <c r="E561" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F561" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F561" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G561" s="9" t="s">
         <v>9</v>
@@ -17547,7 +17568,7 @@
         <v>47</v>
       </c>
       <c r="G562" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.25">
@@ -17735,10 +17756,10 @@
         <v>183</v>
       </c>
       <c r="E572" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F572" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F572" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G572" s="9" t="s">
         <v>9</v>
@@ -17764,7 +17785,7 @@
         <v>36</v>
       </c>
       <c r="G573" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
@@ -17933,10 +17954,10 @@
         <v>183</v>
       </c>
       <c r="E582" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F582" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F582" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G582" s="9" t="s">
         <v>9</v>
@@ -17962,7 +17983,7 @@
         <v>0</v>
       </c>
       <c r="G583" s="50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
@@ -18131,10 +18152,10 @@
         <v>183</v>
       </c>
       <c r="E592" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F592" s="26" t="s">
         <v>393</v>
-      </c>
-      <c r="F592" s="26" t="s">
-        <v>394</v>
       </c>
       <c r="G592" s="9" t="s">
         <v>9</v>
@@ -18160,7 +18181,7 @@
         <v>48</v>
       </c>
       <c r="G593" s="50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
@@ -19801,21 +19822,83 @@
     <row r="2039" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="A530:A538"/>
-    <mergeCell ref="A540:A549"/>
-    <mergeCell ref="A551:A560"/>
-    <mergeCell ref="A562:A571"/>
-    <mergeCell ref="A573:A581"/>
-    <mergeCell ref="A583:A591"/>
-    <mergeCell ref="A593:A600"/>
-    <mergeCell ref="A493:A501"/>
-    <mergeCell ref="A443:A451"/>
-    <mergeCell ref="A453:A461"/>
-    <mergeCell ref="A463:A471"/>
-    <mergeCell ref="A473:A481"/>
-    <mergeCell ref="A483:A491"/>
-    <mergeCell ref="A503:A517"/>
-    <mergeCell ref="A519:A528"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="G45:G54"/>
+    <mergeCell ref="G77:G89"/>
+    <mergeCell ref="G91:G99"/>
+    <mergeCell ref="G56:G64"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="G34:G43"/>
+    <mergeCell ref="G11:G19"/>
+    <mergeCell ref="G21:G32"/>
+    <mergeCell ref="A21:A32"/>
+    <mergeCell ref="A66:A75"/>
+    <mergeCell ref="A91:A99"/>
+    <mergeCell ref="G66:G75"/>
+    <mergeCell ref="A101:A109"/>
+    <mergeCell ref="A77:A89"/>
+    <mergeCell ref="G224:G234"/>
+    <mergeCell ref="G236:G244"/>
+    <mergeCell ref="G200:G211"/>
+    <mergeCell ref="G213:G222"/>
+    <mergeCell ref="G180:G188"/>
+    <mergeCell ref="A180:A188"/>
+    <mergeCell ref="A111:A119"/>
+    <mergeCell ref="G101:G109"/>
+    <mergeCell ref="G121:G129"/>
+    <mergeCell ref="G141:G148"/>
+    <mergeCell ref="G131:G139"/>
+    <mergeCell ref="A236:A244"/>
+    <mergeCell ref="A170:A178"/>
+    <mergeCell ref="G160:G168"/>
+    <mergeCell ref="G190:G198"/>
+    <mergeCell ref="G170:G178"/>
+    <mergeCell ref="A190:A198"/>
+    <mergeCell ref="A200:A211"/>
+    <mergeCell ref="A213:A222"/>
+    <mergeCell ref="G305:G313"/>
+    <mergeCell ref="G266:G274"/>
+    <mergeCell ref="G276:G283"/>
+    <mergeCell ref="G285:G293"/>
+    <mergeCell ref="A266:A274"/>
+    <mergeCell ref="G111:G119"/>
+    <mergeCell ref="A150:A158"/>
+    <mergeCell ref="A141:A148"/>
+    <mergeCell ref="G150:G158"/>
+    <mergeCell ref="G246:G254"/>
+    <mergeCell ref="A246:A254"/>
+    <mergeCell ref="A276:A283"/>
+    <mergeCell ref="A131:A139"/>
+    <mergeCell ref="G256:G264"/>
+    <mergeCell ref="A256:A264"/>
+    <mergeCell ref="A121:A129"/>
+    <mergeCell ref="G295:G303"/>
+    <mergeCell ref="A295:A303"/>
+    <mergeCell ref="A285:A293"/>
+    <mergeCell ref="A224:A234"/>
+    <mergeCell ref="A160:A168"/>
+    <mergeCell ref="G346:G354"/>
+    <mergeCell ref="G356:G364"/>
+    <mergeCell ref="G315:G324"/>
+    <mergeCell ref="G326:G334"/>
+    <mergeCell ref="G336:G344"/>
+    <mergeCell ref="G573:G581"/>
+    <mergeCell ref="G583:G591"/>
+    <mergeCell ref="G593:G600"/>
+    <mergeCell ref="G551:G560"/>
+    <mergeCell ref="G562:G571"/>
+    <mergeCell ref="G384:G391"/>
+    <mergeCell ref="G519:G528"/>
+    <mergeCell ref="G530:G538"/>
+    <mergeCell ref="G540:G549"/>
+    <mergeCell ref="G493:G501"/>
+    <mergeCell ref="G503:G517"/>
+    <mergeCell ref="G411:G419"/>
+    <mergeCell ref="G421:G429"/>
     <mergeCell ref="A336:A344"/>
     <mergeCell ref="A326:A334"/>
     <mergeCell ref="A305:A313"/>
@@ -19840,83 +19923,21 @@
     <mergeCell ref="A402:A409"/>
     <mergeCell ref="A411:A419"/>
     <mergeCell ref="A421:A429"/>
-    <mergeCell ref="G346:G354"/>
-    <mergeCell ref="G356:G364"/>
-    <mergeCell ref="G315:G324"/>
-    <mergeCell ref="G326:G334"/>
-    <mergeCell ref="G336:G344"/>
-    <mergeCell ref="G573:G581"/>
-    <mergeCell ref="G583:G591"/>
-    <mergeCell ref="G593:G600"/>
-    <mergeCell ref="G551:G560"/>
-    <mergeCell ref="G562:G571"/>
-    <mergeCell ref="G384:G391"/>
-    <mergeCell ref="G519:G528"/>
-    <mergeCell ref="G530:G538"/>
-    <mergeCell ref="G540:G549"/>
-    <mergeCell ref="G493:G501"/>
-    <mergeCell ref="G503:G517"/>
-    <mergeCell ref="G411:G419"/>
-    <mergeCell ref="G421:G429"/>
-    <mergeCell ref="G305:G313"/>
-    <mergeCell ref="G266:G274"/>
-    <mergeCell ref="G276:G283"/>
-    <mergeCell ref="G285:G293"/>
-    <mergeCell ref="A266:A274"/>
-    <mergeCell ref="G111:G119"/>
-    <mergeCell ref="A150:A158"/>
-    <mergeCell ref="A141:A148"/>
-    <mergeCell ref="G150:G158"/>
-    <mergeCell ref="G246:G254"/>
-    <mergeCell ref="A246:A254"/>
-    <mergeCell ref="A276:A283"/>
-    <mergeCell ref="A131:A139"/>
-    <mergeCell ref="G256:G264"/>
-    <mergeCell ref="A256:A264"/>
-    <mergeCell ref="A121:A129"/>
-    <mergeCell ref="G295:G303"/>
-    <mergeCell ref="A295:A303"/>
-    <mergeCell ref="A285:A293"/>
-    <mergeCell ref="A224:A234"/>
-    <mergeCell ref="A160:A168"/>
-    <mergeCell ref="A101:A109"/>
-    <mergeCell ref="A77:A89"/>
-    <mergeCell ref="G224:G234"/>
-    <mergeCell ref="G236:G244"/>
-    <mergeCell ref="G200:G211"/>
-    <mergeCell ref="G213:G222"/>
-    <mergeCell ref="G180:G188"/>
-    <mergeCell ref="A180:A188"/>
-    <mergeCell ref="A111:A119"/>
-    <mergeCell ref="G101:G109"/>
-    <mergeCell ref="G121:G129"/>
-    <mergeCell ref="G141:G148"/>
-    <mergeCell ref="G131:G139"/>
-    <mergeCell ref="A236:A244"/>
-    <mergeCell ref="A170:A178"/>
-    <mergeCell ref="G160:G168"/>
-    <mergeCell ref="G190:G198"/>
-    <mergeCell ref="G170:G178"/>
-    <mergeCell ref="A190:A198"/>
-    <mergeCell ref="A200:A211"/>
-    <mergeCell ref="A213:A222"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="G45:G54"/>
-    <mergeCell ref="G77:G89"/>
-    <mergeCell ref="G91:G99"/>
-    <mergeCell ref="G56:G64"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="G34:G43"/>
-    <mergeCell ref="G11:G19"/>
-    <mergeCell ref="G21:G32"/>
-    <mergeCell ref="A21:A32"/>
-    <mergeCell ref="A66:A75"/>
-    <mergeCell ref="A91:A99"/>
-    <mergeCell ref="G66:G75"/>
+    <mergeCell ref="A530:A538"/>
+    <mergeCell ref="A540:A549"/>
+    <mergeCell ref="A551:A560"/>
+    <mergeCell ref="A562:A571"/>
+    <mergeCell ref="A573:A581"/>
+    <mergeCell ref="A583:A591"/>
+    <mergeCell ref="A593:A600"/>
+    <mergeCell ref="A493:A501"/>
+    <mergeCell ref="A443:A451"/>
+    <mergeCell ref="A453:A461"/>
+    <mergeCell ref="A463:A471"/>
+    <mergeCell ref="A473:A481"/>
+    <mergeCell ref="A483:A491"/>
+    <mergeCell ref="A503:A517"/>
+    <mergeCell ref="A519:A528"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A34:A43" r:id="rId1" display="Click here for the 1930 season football articles " xr:uid="{19CFF195-F347-4DC1-882D-E27AE52E410C}"/>
@@ -20023,16 +20044,16 @@
       <c r="D1" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F1" s="64"/>
+      <c r="F1" s="68"/>
       <c r="G1" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="60" t="s">
         <v>182</v>
       </c>
       <c r="B2" s="2">
@@ -20050,12 +20071,12 @@
       <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="57" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="2">
         <v>10152</v>
       </c>
@@ -20071,10 +20092,10 @@
       <c r="F3" s="7">
         <v>12</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="2">
         <v>10156</v>
       </c>
@@ -20090,10 +20111,10 @@
       <c r="F4" s="7">
         <v>14</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="2">
         <v>10171</v>
       </c>
@@ -20109,37 +20130,37 @@
       <c r="F5" s="7">
         <v>23</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="52"/>
+      <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="2"/>
       <c r="C9" s="12" t="s">
         <v>45</v>
@@ -20155,7 +20176,7 @@
         <f>SUM(F2:F8)</f>
         <v>49</v>
       </c>
-      <c r="G9" s="53"/>
+      <c r="G9" s="54"/>
     </row>
     <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
@@ -20170,16 +20191,16 @@
       <c r="D10" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F10" s="64"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="60" t="s">
         <v>184</v>
       </c>
       <c r="B11" s="2">
@@ -20197,12 +20218,12 @@
       <c r="F11" s="7">
         <v>0</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="2">
         <v>10506</v>
       </c>
@@ -20218,10 +20239,10 @@
       <c r="F12" s="7">
         <v>32</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="2">
         <v>10513</v>
       </c>
@@ -20237,10 +20258,10 @@
       <c r="F13" s="7">
         <v>20</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="53"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="2">
         <v>10527</v>
       </c>
@@ -20256,10 +20277,10 @@
       <c r="F14" s="7">
         <v>19</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="2">
         <v>10541</v>
       </c>
@@ -20275,10 +20296,10 @@
       <c r="F15" s="7">
         <v>45</v>
       </c>
-      <c r="G15" s="52"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="2">
         <v>10548</v>
       </c>
@@ -20294,10 +20315,10 @@
       <c r="F16" s="7">
         <v>7</v>
       </c>
-      <c r="G16" s="52"/>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="2">
         <v>10555</v>
       </c>
@@ -20313,10 +20334,10 @@
       <c r="F17" s="7">
         <v>0</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="2">
         <v>10561</v>
       </c>
@@ -20332,10 +20353,10 @@
       <c r="F18" s="7">
         <v>6</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="2"/>
       <c r="C19" s="16" t="s">
         <v>46</v>
@@ -20351,7 +20372,7 @@
         <f>SUM(F11:F18)</f>
         <v>129</v>
       </c>
-      <c r="G19" s="53"/>
+      <c r="G19" s="54"/>
     </row>
     <row r="20" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
@@ -20366,16 +20387,16 @@
       <c r="D20" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F20" s="64"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="61" t="s">
         <v>185</v>
       </c>
       <c r="B21" s="2">
@@ -20393,12 +20414,12 @@
       <c r="F21" s="7">
         <v>27</v>
       </c>
-      <c r="G21" s="51" t="s">
+      <c r="G21" s="57" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="2">
         <v>10870</v>
       </c>
@@ -20414,10 +20435,10 @@
       <c r="F22" s="7">
         <v>13</v>
       </c>
-      <c r="G22" s="52"/>
+      <c r="G22" s="53"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="2">
         <v>10877</v>
       </c>
@@ -20433,10 +20454,10 @@
       <c r="F23" s="7">
         <v>13</v>
       </c>
-      <c r="G23" s="52"/>
+      <c r="G23" s="53"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="2">
         <v>10884</v>
       </c>
@@ -20452,10 +20473,10 @@
       <c r="F24" s="7">
         <v>18</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="53"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="2">
         <v>10891</v>
       </c>
@@ -20471,10 +20492,10 @@
       <c r="F25" s="7">
         <v>24</v>
       </c>
-      <c r="G25" s="52"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="2">
         <v>10898</v>
       </c>
@@ -20490,10 +20511,10 @@
       <c r="F26" s="7">
         <v>7</v>
       </c>
-      <c r="G26" s="52"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="2">
         <v>10905</v>
       </c>
@@ -20509,10 +20530,10 @@
       <c r="F27" s="7">
         <v>0</v>
       </c>
-      <c r="G27" s="52"/>
+      <c r="G27" s="53"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="2">
         <v>10912</v>
       </c>
@@ -20528,10 +20549,10 @@
       <c r="F28" s="7">
         <v>0</v>
       </c>
-      <c r="G28" s="52"/>
+      <c r="G28" s="53"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="2" t="s">
         <v>78</v>
       </c>
@@ -20547,10 +20568,10 @@
       <c r="F29" s="7">
         <v>0</v>
       </c>
-      <c r="G29" s="52"/>
+      <c r="G29" s="53"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="2">
         <v>10917</v>
       </c>
@@ -20566,10 +20587,10 @@
       <c r="F30" s="7">
         <v>0</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="53"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="2">
         <v>10925</v>
       </c>
@@ -20585,10 +20606,10 @@
       <c r="F31" s="7">
         <v>7</v>
       </c>
-      <c r="G31" s="52"/>
+      <c r="G31" s="53"/>
     </row>
     <row r="32" spans="1:7" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16" t="s">
         <v>47</v>
@@ -20604,7 +20625,7 @@
         <f>SUM(F21:F31)</f>
         <v>109</v>
       </c>
-      <c r="G32" s="53"/>
+      <c r="G32" s="54"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
@@ -20619,10 +20640,10 @@
       <c r="D33" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E33" s="63" t="s">
+      <c r="E33" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F33" s="64"/>
+      <c r="F33" s="68"/>
       <c r="G33" s="9" t="s">
         <v>9</v>
       </c>
@@ -20646,7 +20667,7 @@
       <c r="F34" s="7">
         <v>0</v>
       </c>
-      <c r="G34" s="51" t="s">
+      <c r="G34" s="57" t="s">
         <v>252</v>
       </c>
     </row>
@@ -20667,7 +20688,7 @@
       <c r="F35" s="7">
         <v>0</v>
       </c>
-      <c r="G35" s="52"/>
+      <c r="G35" s="53"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="45"/>
@@ -20686,7 +20707,7 @@
       <c r="F36" s="7">
         <v>0</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="53"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
@@ -20705,7 +20726,7 @@
       <c r="F37" s="7">
         <v>0</v>
       </c>
-      <c r="G37" s="52"/>
+      <c r="G37" s="53"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="45"/>
@@ -20724,7 +20745,7 @@
       <c r="F38" s="7">
         <v>6</v>
       </c>
-      <c r="G38" s="52"/>
+      <c r="G38" s="53"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
@@ -20743,7 +20764,7 @@
       <c r="F39" s="7">
         <v>0</v>
       </c>
-      <c r="G39" s="52"/>
+      <c r="G39" s="53"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="45"/>
@@ -20762,7 +20783,7 @@
       <c r="F40" s="7">
         <v>0</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="53"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="45"/>
@@ -20781,7 +20802,7 @@
       <c r="F41" s="7">
         <v>0</v>
       </c>
-      <c r="G41" s="52"/>
+      <c r="G41" s="53"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="45"/>
@@ -20800,7 +20821,7 @@
       <c r="F42" s="7">
         <v>0</v>
       </c>
-      <c r="G42" s="52"/>
+      <c r="G42" s="53"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="46"/>
@@ -20819,7 +20840,7 @@
         <f>SUM(F34:F42)</f>
         <v>6</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="54"/>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
@@ -20834,16 +20855,16 @@
       <c r="D44" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E44" s="63" t="s">
+      <c r="E44" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F44" s="64"/>
+      <c r="F44" s="68"/>
       <c r="G44" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47" t="s">
+      <c r="A45" s="59" t="s">
         <v>187</v>
       </c>
       <c r="B45" s="2">
@@ -21030,10 +21051,10 @@
       <c r="D54" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E54" s="63" t="s">
+      <c r="E54" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F54" s="64"/>
+      <c r="F54" s="68"/>
       <c r="G54" s="9" t="s">
         <v>9</v>
       </c>
@@ -21444,7 +21465,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="58" t="s">
+      <c r="A76" s="55" t="s">
         <v>190</v>
       </c>
       <c r="B76" s="2">
@@ -21462,12 +21483,12 @@
       <c r="F76" s="7">
         <v>6</v>
       </c>
-      <c r="G76" s="51" t="s">
+      <c r="G76" s="57" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="57"/>
+      <c r="A77" s="56"/>
       <c r="B77" s="2">
         <v>12699</v>
       </c>
@@ -21483,10 +21504,10 @@
       <c r="F77" s="7">
         <v>12</v>
       </c>
-      <c r="G77" s="52"/>
+      <c r="G77" s="53"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="57"/>
+      <c r="A78" s="56"/>
       <c r="B78" s="2">
         <v>12705</v>
       </c>
@@ -21502,10 +21523,10 @@
       <c r="F78" s="7">
         <v>15</v>
       </c>
-      <c r="G78" s="52"/>
+      <c r="G78" s="53"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="57"/>
+      <c r="A79" s="56"/>
       <c r="B79" s="2">
         <v>12713</v>
       </c>
@@ -21521,10 +21542,10 @@
       <c r="F79" s="7">
         <v>0</v>
       </c>
-      <c r="G79" s="52"/>
+      <c r="G79" s="53"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="57"/>
+      <c r="A80" s="56"/>
       <c r="B80" s="2">
         <v>12720</v>
       </c>
@@ -21540,10 +21561,10 @@
       <c r="F80" s="7">
         <v>0</v>
       </c>
-      <c r="G80" s="52"/>
+      <c r="G80" s="53"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="57"/>
+      <c r="A81" s="56"/>
       <c r="B81" s="2">
         <v>12727</v>
       </c>
@@ -21559,10 +21580,10 @@
       <c r="F81" s="7">
         <v>0</v>
       </c>
-      <c r="G81" s="52"/>
+      <c r="G81" s="53"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="57"/>
+      <c r="A82" s="56"/>
       <c r="B82" s="40">
         <v>12734</v>
       </c>
@@ -21578,10 +21599,10 @@
       <c r="F82" s="43">
         <v>0</v>
       </c>
-      <c r="G82" s="52"/>
+      <c r="G82" s="53"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="57"/>
+      <c r="A83" s="56"/>
       <c r="B83" s="2">
         <v>12741</v>
       </c>
@@ -21597,18 +21618,18 @@
       <c r="F83" s="7">
         <v>0</v>
       </c>
-      <c r="G83" s="52"/>
+      <c r="G83" s="53"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="57"/>
+      <c r="A84" s="56"/>
       <c r="B84" s="2"/>
       <c r="D84" s="3"/>
       <c r="E84" s="6"/>
       <c r="F84" s="7"/>
-      <c r="G84" s="52"/>
+      <c r="G84" s="53"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="57"/>
+      <c r="A85" s="56"/>
       <c r="B85" s="3"/>
       <c r="C85" s="20" t="s">
         <v>13</v>
@@ -21622,10 +21643,10 @@
       <c r="F85" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G85" s="52"/>
+      <c r="G85" s="53"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="57"/>
+      <c r="A86" s="56"/>
       <c r="B86" s="35"/>
       <c r="C86" s="39" t="s">
         <v>42</v>
@@ -21633,10 +21654,10 @@
       <c r="D86" s="36"/>
       <c r="E86" s="37"/>
       <c r="F86" s="38"/>
-      <c r="G86" s="52"/>
+      <c r="G86" s="53"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="57"/>
+      <c r="A87" s="56"/>
       <c r="B87" s="35"/>
       <c r="C87" s="20" t="s">
         <v>43</v>
@@ -21652,7 +21673,7 @@
         <f>SUM(F76:F86)</f>
         <v>33</v>
       </c>
-      <c r="G87" s="53"/>
+      <c r="G87" s="54"/>
     </row>
     <row r="88" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
@@ -21676,7 +21697,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="57" t="s">
+      <c r="A89" s="56" t="s">
         <v>191</v>
       </c>
       <c r="B89" s="2">
@@ -21699,7 +21720,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="57"/>
+      <c r="A90" s="56"/>
       <c r="B90" s="2">
         <v>13069</v>
       </c>
@@ -21718,7 +21739,7 @@
       <c r="G90" s="50"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="57"/>
+      <c r="A91" s="56"/>
       <c r="B91" s="2">
         <v>13077</v>
       </c>
@@ -21737,7 +21758,7 @@
       <c r="G91" s="50"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="57"/>
+      <c r="A92" s="56"/>
       <c r="B92" s="2">
         <v>13084</v>
       </c>
@@ -21756,7 +21777,7 @@
       <c r="G92" s="50"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="57"/>
+      <c r="A93" s="56"/>
       <c r="B93" s="2">
         <v>13091</v>
       </c>
@@ -21775,7 +21796,7 @@
       <c r="G93" s="50"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="57"/>
+      <c r="A94" s="56"/>
       <c r="B94" s="2">
         <v>13098</v>
       </c>
@@ -21794,7 +21815,7 @@
       <c r="G94" s="50"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="57"/>
+      <c r="A95" s="56"/>
       <c r="B95" s="2">
         <v>13105</v>
       </c>
@@ -21813,7 +21834,7 @@
       <c r="G95" s="50"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="57"/>
+      <c r="A96" s="56"/>
       <c r="B96" s="2">
         <v>13112</v>
       </c>
@@ -21832,7 +21853,7 @@
       <c r="G96" s="50"/>
     </row>
     <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="57"/>
+      <c r="A97" s="56"/>
       <c r="B97" s="3"/>
       <c r="C97" s="20" t="s">
         <v>44</v>
@@ -22820,10 +22841,10 @@
       <c r="D147" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E147" s="67" t="s">
+      <c r="E147" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F147" s="68"/>
+      <c r="F147" s="64"/>
       <c r="G147" s="9" t="s">
         <v>9</v>
       </c>
@@ -22847,7 +22868,7 @@
       <c r="F148" s="7">
         <v>12</v>
       </c>
-      <c r="G148" s="61" t="s">
+      <c r="G148" s="52" t="s">
         <v>267</v>
       </c>
     </row>
@@ -22868,7 +22889,7 @@
       <c r="F149" s="7">
         <v>0</v>
       </c>
-      <c r="G149" s="52"/>
+      <c r="G149" s="53"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="45"/>
@@ -22887,7 +22908,7 @@
       <c r="F150" s="7">
         <v>13</v>
       </c>
-      <c r="G150" s="52"/>
+      <c r="G150" s="53"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="45"/>
@@ -22906,7 +22927,7 @@
       <c r="F151" s="7">
         <v>0</v>
       </c>
-      <c r="G151" s="52"/>
+      <c r="G151" s="53"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="45"/>
@@ -22925,7 +22946,7 @@
       <c r="F152" s="7">
         <v>31</v>
       </c>
-      <c r="G152" s="52"/>
+      <c r="G152" s="53"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="45"/>
@@ -22944,7 +22965,7 @@
       <c r="F153" s="7">
         <v>13</v>
       </c>
-      <c r="G153" s="52"/>
+      <c r="G153" s="53"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="45"/>
@@ -22963,7 +22984,7 @@
       <c r="F154" s="7">
         <v>21</v>
       </c>
-      <c r="G154" s="52"/>
+      <c r="G154" s="53"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="45"/>
@@ -22982,7 +23003,7 @@
       <c r="F155" s="7">
         <v>38</v>
       </c>
-      <c r="G155" s="52"/>
+      <c r="G155" s="53"/>
     </row>
     <row r="156" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="46"/>
@@ -23001,7 +23022,7 @@
         <f>SUM(F148:F155)</f>
         <v>128</v>
       </c>
-      <c r="G156" s="53"/>
+      <c r="G156" s="54"/>
     </row>
     <row r="157" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="28" t="s">
@@ -23016,10 +23037,10 @@
       <c r="D157" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E157" s="67" t="s">
+      <c r="E157" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F157" s="68"/>
+      <c r="F157" s="64"/>
       <c r="G157" s="9" t="s">
         <v>9</v>
       </c>
@@ -23043,7 +23064,7 @@
       <c r="F158" s="5">
         <v>7</v>
       </c>
-      <c r="G158" s="60" t="s">
+      <c r="G158" s="51" t="s">
         <v>269</v>
       </c>
     </row>
@@ -23206,10 +23227,10 @@
       <c r="D167" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E167" s="67" t="s">
+      <c r="E167" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F167" s="68"/>
+      <c r="F167" s="64"/>
       <c r="G167" s="9" t="s">
         <v>9</v>
       </c>
@@ -23233,7 +23254,7 @@
       <c r="F168" s="5">
         <v>12</v>
       </c>
-      <c r="G168" s="60" t="s">
+      <c r="G168" s="51" t="s">
         <v>271</v>
       </c>
     </row>
@@ -23402,10 +23423,10 @@
       <c r="D177" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E177" s="67" t="s">
+      <c r="E177" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F177" s="68"/>
+      <c r="F177" s="64"/>
       <c r="G177" s="9" t="s">
         <v>9</v>
       </c>
@@ -23598,10 +23619,10 @@
       <c r="D187" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E187" s="67" t="s">
+      <c r="E187" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F187" s="68"/>
+      <c r="F187" s="64"/>
       <c r="G187" s="9" t="s">
         <v>9</v>
       </c>
@@ -23625,7 +23646,7 @@
       <c r="F188" s="5">
         <v>26</v>
       </c>
-      <c r="G188" s="60" t="s">
+      <c r="G188" s="51" t="s">
         <v>274</v>
       </c>
     </row>
@@ -23794,16 +23815,16 @@
       <c r="D197" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E197" s="67" t="s">
+      <c r="E197" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F197" s="68"/>
+      <c r="F197" s="64"/>
       <c r="G197" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A198" s="47" t="s">
+      <c r="A198" s="59" t="s">
         <v>202</v>
       </c>
       <c r="B198" s="2">
@@ -23821,7 +23842,7 @@
       <c r="F198" s="5">
         <v>7</v>
       </c>
-      <c r="G198" s="59" t="s">
+      <c r="G198" s="58" t="s">
         <v>276</v>
       </c>
     </row>
@@ -23975,7 +23996,7 @@
       <c r="F206" s="5">
         <v>7</v>
       </c>
-      <c r="G206" s="51"/>
+      <c r="G206" s="57"/>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="48"/>
@@ -23984,7 +24005,7 @@
       <c r="D207" s="3"/>
       <c r="E207" s="8"/>
       <c r="F207" s="5"/>
-      <c r="G207" s="51"/>
+      <c r="G207" s="57"/>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="48"/>
@@ -23993,7 +24014,7 @@
       <c r="D208" s="3"/>
       <c r="E208" s="8"/>
       <c r="F208" s="5"/>
-      <c r="G208" s="51"/>
+      <c r="G208" s="57"/>
     </row>
     <row r="209" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="49"/>
@@ -24012,7 +24033,7 @@
         <f>SUM(F198:F206)</f>
         <v>16</v>
       </c>
-      <c r="G209" s="51"/>
+      <c r="G209" s="57"/>
     </row>
     <row r="210" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="28" t="s">
@@ -24027,10 +24048,10 @@
       <c r="D210" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E210" s="67" t="s">
+      <c r="E210" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F210" s="68"/>
+      <c r="F210" s="64"/>
       <c r="G210" s="9" t="s">
         <v>9</v>
       </c>
@@ -24054,7 +24075,7 @@
       <c r="F211" s="7">
         <v>13</v>
       </c>
-      <c r="G211" s="60" t="s">
+      <c r="G211" s="51" t="s">
         <v>277</v>
       </c>
     </row>
@@ -24242,16 +24263,16 @@
       <c r="D221" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E221" s="67" t="s">
+      <c r="E221" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F221" s="68"/>
+      <c r="F221" s="64"/>
       <c r="G221" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A222" s="58" t="s">
+      <c r="A222" s="55" t="s">
         <v>204</v>
       </c>
       <c r="B222" s="2">
@@ -24274,7 +24295,7 @@
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="57"/>
+      <c r="A223" s="56"/>
       <c r="B223" s="2">
         <v>17802</v>
       </c>
@@ -24293,7 +24314,7 @@
       <c r="G223" s="50"/>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A224" s="57"/>
+      <c r="A224" s="56"/>
       <c r="B224" s="4">
         <v>17809</v>
       </c>
@@ -24312,7 +24333,7 @@
       <c r="G224" s="50"/>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225" s="57"/>
+      <c r="A225" s="56"/>
       <c r="B225" s="2">
         <v>17814</v>
       </c>
@@ -24331,7 +24352,7 @@
       <c r="G225" s="50"/>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" s="57"/>
+      <c r="A226" s="56"/>
       <c r="B226" s="2">
         <v>17822</v>
       </c>
@@ -24350,7 +24371,7 @@
       <c r="G226" s="50"/>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A227" s="57"/>
+      <c r="A227" s="56"/>
       <c r="B227" s="2">
         <v>17830</v>
       </c>
@@ -24369,7 +24390,7 @@
       <c r="G227" s="50"/>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A228" s="57"/>
+      <c r="A228" s="56"/>
       <c r="B228" s="2">
         <v>17844</v>
       </c>
@@ -24388,7 +24409,7 @@
       <c r="G228" s="50"/>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A229" s="57"/>
+      <c r="A229" s="56"/>
       <c r="B229" s="4">
         <v>17852</v>
       </c>
@@ -24407,7 +24428,7 @@
       <c r="G229" s="50"/>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="57"/>
+      <c r="A230" s="56"/>
       <c r="B230" s="4"/>
       <c r="C230" s="3"/>
       <c r="D230" s="3"/>
@@ -24416,7 +24437,7 @@
       <c r="G230" s="50"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="57"/>
+      <c r="A231" s="56"/>
       <c r="B231" s="4"/>
       <c r="C231" s="3"/>
       <c r="D231" s="3"/>
@@ -24425,7 +24446,7 @@
       <c r="G231" s="50"/>
     </row>
     <row r="232" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="57"/>
+      <c r="A232" s="56"/>
       <c r="B232" s="3"/>
       <c r="C232" s="20" t="s">
         <v>139</v>
@@ -24456,10 +24477,10 @@
       <c r="D233" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E233" s="67" t="s">
+      <c r="E233" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F233" s="68"/>
+      <c r="F233" s="64"/>
       <c r="G233" s="9" t="s">
         <v>9</v>
       </c>
@@ -24637,7 +24658,7 @@
         <f>SUM(F234:F241)</f>
         <v>82</v>
       </c>
-      <c r="G242" s="51"/>
+      <c r="G242" s="57"/>
     </row>
     <row r="243" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="28" t="s">
@@ -24652,10 +24673,10 @@
       <c r="D243" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E243" s="67" t="s">
+      <c r="E243" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F243" s="68"/>
+      <c r="F243" s="64"/>
       <c r="G243" s="9" t="s">
         <v>9</v>
       </c>
@@ -24679,7 +24700,7 @@
       <c r="F244" s="5">
         <v>31</v>
       </c>
-      <c r="G244" s="60" t="s">
+      <c r="G244" s="51" t="s">
         <v>280</v>
       </c>
     </row>
@@ -24848,10 +24869,10 @@
       <c r="D253" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E253" s="67" t="s">
+      <c r="E253" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F253" s="68"/>
+      <c r="F253" s="64"/>
       <c r="G253" s="9" t="s">
         <v>9</v>
       </c>
@@ -25044,10 +25065,10 @@
       <c r="D263" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E263" s="67" t="s">
+      <c r="E263" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F263" s="68"/>
+      <c r="F263" s="64"/>
       <c r="G263" s="9" t="s">
         <v>9</v>
       </c>
@@ -25236,10 +25257,10 @@
       <c r="D273" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E273" s="67" t="s">
+      <c r="E273" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F273" s="68"/>
+      <c r="F273" s="64"/>
       <c r="G273" s="9" t="s">
         <v>9</v>
       </c>
@@ -25413,10 +25434,10 @@
       <c r="D282" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E282" s="67" t="s">
+      <c r="E282" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F282" s="68"/>
+      <c r="F282" s="64"/>
       <c r="G282" s="9" t="s">
         <v>9</v>
       </c>
@@ -25440,7 +25461,7 @@
       <c r="F283" s="7">
         <v>19</v>
       </c>
-      <c r="G283" s="60" t="s">
+      <c r="G283" s="51" t="s">
         <v>287</v>
       </c>
     </row>
@@ -25609,10 +25630,10 @@
       <c r="D292" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E292" s="67" t="s">
+      <c r="E292" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F292" s="68"/>
+      <c r="F292" s="64"/>
       <c r="G292" s="9" t="s">
         <v>9</v>
       </c>
@@ -25805,10 +25826,10 @@
       <c r="D302" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E302" s="67" t="s">
+      <c r="E302" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F302" s="68"/>
+      <c r="F302" s="64"/>
       <c r="G302" s="9" t="s">
         <v>9</v>
       </c>
@@ -25832,7 +25853,7 @@
       <c r="F303" s="5">
         <v>12</v>
       </c>
-      <c r="G303" s="60" t="s">
+      <c r="G303" s="51" t="s">
         <v>290</v>
       </c>
     </row>
@@ -26001,10 +26022,10 @@
       <c r="D312" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E312" s="67" t="s">
+      <c r="E312" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F312" s="68"/>
+      <c r="F312" s="64"/>
       <c r="G312" s="9" t="s">
         <v>9</v>
       </c>
@@ -26208,10 +26229,10 @@
       <c r="D323" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E323" s="67" t="s">
+      <c r="E323" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F323" s="68"/>
+      <c r="F323" s="64"/>
       <c r="G323" s="9" t="s">
         <v>9</v>
       </c>
@@ -26404,10 +26425,10 @@
       <c r="D333" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E333" s="67" t="s">
+      <c r="E333" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F333" s="68"/>
+      <c r="F333" s="64"/>
       <c r="G333" s="9" t="s">
         <v>9</v>
       </c>
@@ -26600,10 +26621,10 @@
       <c r="D343" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E343" s="67" t="s">
+      <c r="E343" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F343" s="68"/>
+      <c r="F343" s="64"/>
       <c r="G343" s="9" t="s">
         <v>9</v>
       </c>
@@ -26796,10 +26817,10 @@
       <c r="D353" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E353" s="67" t="s">
+      <c r="E353" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F353" s="68"/>
+      <c r="F353" s="64"/>
       <c r="G353" s="9" t="s">
         <v>9</v>
       </c>
@@ -26992,10 +27013,10 @@
       <c r="D363" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E363" s="67" t="s">
+      <c r="E363" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F363" s="68"/>
+      <c r="F363" s="64"/>
       <c r="G363" s="9" t="s">
         <v>9</v>
       </c>
@@ -27169,10 +27190,10 @@
       <c r="D372" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E372" s="67" t="s">
+      <c r="E372" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F372" s="68"/>
+      <c r="F372" s="64"/>
       <c r="G372" s="9" t="s">
         <v>9</v>
       </c>
@@ -27346,10 +27367,10 @@
       <c r="D381" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E381" s="67" t="s">
+      <c r="E381" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F381" s="68"/>
+      <c r="F381" s="64"/>
       <c r="G381" s="9" t="s">
         <v>9</v>
       </c>
@@ -27523,10 +27544,10 @@
       <c r="D390" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E390" s="67" t="s">
+      <c r="E390" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F390" s="68"/>
+      <c r="F390" s="64"/>
       <c r="G390" s="9" t="s">
         <v>9</v>
       </c>
@@ -27700,10 +27721,10 @@
       <c r="D399" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E399" s="67" t="s">
+      <c r="E399" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F399" s="68"/>
+      <c r="F399" s="64"/>
       <c r="G399" s="9" t="s">
         <v>9</v>
       </c>
@@ -27877,10 +27898,10 @@
       <c r="D408" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E408" s="67" t="s">
+      <c r="E408" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F408" s="68"/>
+      <c r="F408" s="64"/>
       <c r="G408" s="9" t="s">
         <v>9</v>
       </c>
@@ -28073,10 +28094,10 @@
       <c r="D418" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E418" s="67" t="s">
+      <c r="E418" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F418" s="68"/>
+      <c r="F418" s="64"/>
       <c r="G418" s="9" t="s">
         <v>9</v>
       </c>
@@ -28271,10 +28292,10 @@
       <c r="D428" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E428" s="67" t="s">
+      <c r="E428" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F428" s="68"/>
+      <c r="F428" s="64"/>
       <c r="G428" s="9" t="s">
         <v>9</v>
       </c>
@@ -28485,10 +28506,10 @@
       <c r="D440" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E440" s="67" t="s">
+      <c r="E440" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F440" s="68"/>
+      <c r="F440" s="64"/>
       <c r="G440" s="9" t="s">
         <v>9</v>
       </c>
@@ -28681,10 +28702,10 @@
       <c r="D450" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E450" s="67" t="s">
+      <c r="E450" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F450" s="68"/>
+      <c r="F450" s="64"/>
       <c r="G450" s="9" t="s">
         <v>179</v>
       </c>
@@ -28877,10 +28898,10 @@
       <c r="D460" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E460" s="67" t="s">
+      <c r="E460" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F460" s="68"/>
+      <c r="F460" s="64"/>
       <c r="G460" s="9" t="s">
         <v>9</v>
       </c>
@@ -29073,10 +29094,10 @@
       <c r="D470" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E470" s="67" t="s">
+      <c r="E470" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F470" s="68"/>
+      <c r="F470" s="64"/>
       <c r="G470" s="9" t="s">
         <v>9</v>
       </c>
@@ -29100,7 +29121,7 @@
       <c r="F471" s="5">
         <v>19</v>
       </c>
-      <c r="G471" s="60" t="s">
+      <c r="G471" s="51" t="s">
         <v>314</v>
       </c>
     </row>
@@ -29269,10 +29290,10 @@
       <c r="D480" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E480" s="67" t="s">
+      <c r="E480" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F480" s="68"/>
+      <c r="F480" s="64"/>
       <c r="G480" s="9" t="s">
         <v>9</v>
       </c>
@@ -29465,10 +29486,10 @@
       <c r="D490" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E490" s="67" t="s">
+      <c r="E490" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F490" s="68"/>
+      <c r="F490" s="64"/>
       <c r="G490" s="9" t="s">
         <v>9</v>
       </c>
@@ -29661,16 +29682,16 @@
       <c r="D500" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E500" s="67" t="s">
+      <c r="E500" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F500" s="68"/>
+      <c r="F500" s="64"/>
       <c r="G500" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A501" s="62" t="s">
+      <c r="A501" s="47" t="s">
         <v>232</v>
       </c>
       <c r="B501" s="2">
@@ -29912,10 +29933,10 @@
       <c r="D515" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E515" s="67" t="s">
+      <c r="E515" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F515" s="68"/>
+      <c r="F515" s="64"/>
       <c r="G515" s="9" t="s">
         <v>9</v>
       </c>
@@ -30127,10 +30148,10 @@
       <c r="D526" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E526" s="67" t="s">
+      <c r="E526" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F526" s="68"/>
+      <c r="F526" s="64"/>
       <c r="G526" s="9" t="s">
         <v>9</v>
       </c>
@@ -30323,10 +30344,10 @@
       <c r="D536" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E536" s="67" t="s">
+      <c r="E536" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F536" s="68"/>
+      <c r="F536" s="64"/>
       <c r="G536" s="9" t="s">
         <v>9</v>
       </c>
@@ -30538,10 +30559,10 @@
       <c r="D547" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E547" s="67" t="s">
+      <c r="E547" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F547" s="68"/>
+      <c r="F547" s="64"/>
       <c r="G547" s="9" t="s">
         <v>9</v>
       </c>
@@ -30753,10 +30774,10 @@
       <c r="D558" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E558" s="67" t="s">
+      <c r="E558" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F558" s="68"/>
+      <c r="F558" s="64"/>
       <c r="G558" s="9" t="s">
         <v>9</v>
       </c>
@@ -30968,10 +30989,10 @@
       <c r="D569" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E569" s="67" t="s">
+      <c r="E569" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F569" s="68"/>
+      <c r="F569" s="64"/>
       <c r="G569" s="9" t="s">
         <v>9</v>
       </c>
@@ -31164,10 +31185,10 @@
       <c r="D579" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E579" s="67" t="s">
+      <c r="E579" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F579" s="68"/>
+      <c r="F579" s="64"/>
       <c r="G579" s="9" t="s">
         <v>9</v>
       </c>
@@ -31360,10 +31381,10 @@
       <c r="D589" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E589" s="67" t="s">
+      <c r="E589" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F589" s="68"/>
+      <c r="F589" s="64"/>
       <c r="G589" s="9" t="s">
         <v>9</v>
       </c>
@@ -33053,6 +33074,168 @@
     <row r="2036" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="174">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="G11:G19"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="A45:A53"/>
+    <mergeCell ref="G45:G53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="A55:A63"/>
+    <mergeCell ref="G55:G63"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A21:A32"/>
+    <mergeCell ref="G21:G32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="G34:G43"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="A89:A97"/>
+    <mergeCell ref="G89:G97"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="A99:A107"/>
+    <mergeCell ref="G99:G107"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:A74"/>
+    <mergeCell ref="G65:G74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="A76:A87"/>
+    <mergeCell ref="G76:G87"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="A129:A137"/>
+    <mergeCell ref="G129:G137"/>
+    <mergeCell ref="E138:F138"/>
+    <mergeCell ref="A139:A146"/>
+    <mergeCell ref="G139:G146"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="A109:A117"/>
+    <mergeCell ref="G109:G117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="A119:A127"/>
+    <mergeCell ref="G119:G127"/>
+    <mergeCell ref="E167:F167"/>
+    <mergeCell ref="A168:A176"/>
+    <mergeCell ref="G168:G176"/>
+    <mergeCell ref="E177:F177"/>
+    <mergeCell ref="A178:A186"/>
+    <mergeCell ref="G178:G186"/>
+    <mergeCell ref="E147:F147"/>
+    <mergeCell ref="A148:A156"/>
+    <mergeCell ref="G148:G156"/>
+    <mergeCell ref="E157:F157"/>
+    <mergeCell ref="A158:A166"/>
+    <mergeCell ref="G158:G166"/>
+    <mergeCell ref="E210:F210"/>
+    <mergeCell ref="A211:A220"/>
+    <mergeCell ref="G211:G220"/>
+    <mergeCell ref="E221:F221"/>
+    <mergeCell ref="A222:A232"/>
+    <mergeCell ref="G222:G232"/>
+    <mergeCell ref="E187:F187"/>
+    <mergeCell ref="A188:A196"/>
+    <mergeCell ref="G188:G196"/>
+    <mergeCell ref="E197:F197"/>
+    <mergeCell ref="A198:A209"/>
+    <mergeCell ref="G198:G209"/>
+    <mergeCell ref="E253:F253"/>
+    <mergeCell ref="A254:A262"/>
+    <mergeCell ref="G254:G262"/>
+    <mergeCell ref="E263:F263"/>
+    <mergeCell ref="A264:A272"/>
+    <mergeCell ref="G264:G272"/>
+    <mergeCell ref="E233:F233"/>
+    <mergeCell ref="A234:A242"/>
+    <mergeCell ref="G234:G242"/>
+    <mergeCell ref="E243:F243"/>
+    <mergeCell ref="A244:A252"/>
+    <mergeCell ref="G244:G252"/>
+    <mergeCell ref="E292:F292"/>
+    <mergeCell ref="A293:A301"/>
+    <mergeCell ref="G293:G301"/>
+    <mergeCell ref="E302:F302"/>
+    <mergeCell ref="A303:A311"/>
+    <mergeCell ref="G303:G311"/>
+    <mergeCell ref="E273:F273"/>
+    <mergeCell ref="A274:A281"/>
+    <mergeCell ref="G274:G281"/>
+    <mergeCell ref="E282:F282"/>
+    <mergeCell ref="A283:A291"/>
+    <mergeCell ref="G283:G291"/>
+    <mergeCell ref="E333:F333"/>
+    <mergeCell ref="A334:A342"/>
+    <mergeCell ref="G334:G342"/>
+    <mergeCell ref="E343:F343"/>
+    <mergeCell ref="A344:A352"/>
+    <mergeCell ref="G344:G352"/>
+    <mergeCell ref="E312:F312"/>
+    <mergeCell ref="A313:A322"/>
+    <mergeCell ref="G313:G322"/>
+    <mergeCell ref="E323:F323"/>
+    <mergeCell ref="A324:A332"/>
+    <mergeCell ref="G324:G332"/>
+    <mergeCell ref="E372:F372"/>
+    <mergeCell ref="A373:A380"/>
+    <mergeCell ref="G373:G380"/>
+    <mergeCell ref="E381:F381"/>
+    <mergeCell ref="A382:A389"/>
+    <mergeCell ref="G382:G389"/>
+    <mergeCell ref="E353:F353"/>
+    <mergeCell ref="A354:A362"/>
+    <mergeCell ref="G354:G362"/>
+    <mergeCell ref="E363:F363"/>
+    <mergeCell ref="A364:A371"/>
+    <mergeCell ref="G364:G371"/>
+    <mergeCell ref="E408:F408"/>
+    <mergeCell ref="A409:A417"/>
+    <mergeCell ref="G409:G417"/>
+    <mergeCell ref="E418:F418"/>
+    <mergeCell ref="A419:A427"/>
+    <mergeCell ref="G419:G427"/>
+    <mergeCell ref="E390:F390"/>
+    <mergeCell ref="A391:A398"/>
+    <mergeCell ref="G391:G398"/>
+    <mergeCell ref="E399:F399"/>
+    <mergeCell ref="A400:A407"/>
+    <mergeCell ref="G400:G407"/>
+    <mergeCell ref="E450:F450"/>
+    <mergeCell ref="A451:A459"/>
+    <mergeCell ref="G451:G459"/>
+    <mergeCell ref="E460:F460"/>
+    <mergeCell ref="A461:A469"/>
+    <mergeCell ref="G461:G469"/>
+    <mergeCell ref="E428:F428"/>
+    <mergeCell ref="A429:A439"/>
+    <mergeCell ref="G429:G439"/>
+    <mergeCell ref="E440:F440"/>
+    <mergeCell ref="A441:A449"/>
+    <mergeCell ref="G441:G449"/>
+    <mergeCell ref="E490:F490"/>
+    <mergeCell ref="A491:A499"/>
+    <mergeCell ref="G491:G499"/>
+    <mergeCell ref="E500:F500"/>
+    <mergeCell ref="A501:A514"/>
+    <mergeCell ref="G501:G514"/>
+    <mergeCell ref="E470:F470"/>
+    <mergeCell ref="A471:A479"/>
+    <mergeCell ref="G471:G479"/>
+    <mergeCell ref="E480:F480"/>
+    <mergeCell ref="A481:A489"/>
+    <mergeCell ref="G481:G489"/>
+    <mergeCell ref="E536:F536"/>
+    <mergeCell ref="A537:A546"/>
+    <mergeCell ref="G537:G546"/>
+    <mergeCell ref="E547:F547"/>
+    <mergeCell ref="A548:A557"/>
+    <mergeCell ref="G548:G557"/>
+    <mergeCell ref="E515:F515"/>
+    <mergeCell ref="A516:A525"/>
+    <mergeCell ref="G516:G525"/>
+    <mergeCell ref="E526:F526"/>
+    <mergeCell ref="A527:A535"/>
+    <mergeCell ref="G527:G535"/>
     <mergeCell ref="E579:F579"/>
     <mergeCell ref="A580:A588"/>
     <mergeCell ref="G580:G588"/>
@@ -33065,168 +33248,6 @@
     <mergeCell ref="E569:F569"/>
     <mergeCell ref="A570:A578"/>
     <mergeCell ref="G570:G578"/>
-    <mergeCell ref="E536:F536"/>
-    <mergeCell ref="A537:A546"/>
-    <mergeCell ref="G537:G546"/>
-    <mergeCell ref="E547:F547"/>
-    <mergeCell ref="A548:A557"/>
-    <mergeCell ref="G548:G557"/>
-    <mergeCell ref="E515:F515"/>
-    <mergeCell ref="A516:A525"/>
-    <mergeCell ref="G516:G525"/>
-    <mergeCell ref="E526:F526"/>
-    <mergeCell ref="A527:A535"/>
-    <mergeCell ref="G527:G535"/>
-    <mergeCell ref="E490:F490"/>
-    <mergeCell ref="A491:A499"/>
-    <mergeCell ref="G491:G499"/>
-    <mergeCell ref="E500:F500"/>
-    <mergeCell ref="A501:A514"/>
-    <mergeCell ref="G501:G514"/>
-    <mergeCell ref="E470:F470"/>
-    <mergeCell ref="A471:A479"/>
-    <mergeCell ref="G471:G479"/>
-    <mergeCell ref="E480:F480"/>
-    <mergeCell ref="A481:A489"/>
-    <mergeCell ref="G481:G489"/>
-    <mergeCell ref="E450:F450"/>
-    <mergeCell ref="A451:A459"/>
-    <mergeCell ref="G451:G459"/>
-    <mergeCell ref="E460:F460"/>
-    <mergeCell ref="A461:A469"/>
-    <mergeCell ref="G461:G469"/>
-    <mergeCell ref="E428:F428"/>
-    <mergeCell ref="A429:A439"/>
-    <mergeCell ref="G429:G439"/>
-    <mergeCell ref="E440:F440"/>
-    <mergeCell ref="A441:A449"/>
-    <mergeCell ref="G441:G449"/>
-    <mergeCell ref="E408:F408"/>
-    <mergeCell ref="A409:A417"/>
-    <mergeCell ref="G409:G417"/>
-    <mergeCell ref="E418:F418"/>
-    <mergeCell ref="A419:A427"/>
-    <mergeCell ref="G419:G427"/>
-    <mergeCell ref="E390:F390"/>
-    <mergeCell ref="A391:A398"/>
-    <mergeCell ref="G391:G398"/>
-    <mergeCell ref="E399:F399"/>
-    <mergeCell ref="A400:A407"/>
-    <mergeCell ref="G400:G407"/>
-    <mergeCell ref="E372:F372"/>
-    <mergeCell ref="A373:A380"/>
-    <mergeCell ref="G373:G380"/>
-    <mergeCell ref="E381:F381"/>
-    <mergeCell ref="A382:A389"/>
-    <mergeCell ref="G382:G389"/>
-    <mergeCell ref="E353:F353"/>
-    <mergeCell ref="A354:A362"/>
-    <mergeCell ref="G354:G362"/>
-    <mergeCell ref="E363:F363"/>
-    <mergeCell ref="A364:A371"/>
-    <mergeCell ref="G364:G371"/>
-    <mergeCell ref="E333:F333"/>
-    <mergeCell ref="A334:A342"/>
-    <mergeCell ref="G334:G342"/>
-    <mergeCell ref="E343:F343"/>
-    <mergeCell ref="A344:A352"/>
-    <mergeCell ref="G344:G352"/>
-    <mergeCell ref="E312:F312"/>
-    <mergeCell ref="A313:A322"/>
-    <mergeCell ref="G313:G322"/>
-    <mergeCell ref="E323:F323"/>
-    <mergeCell ref="A324:A332"/>
-    <mergeCell ref="G324:G332"/>
-    <mergeCell ref="E292:F292"/>
-    <mergeCell ref="A293:A301"/>
-    <mergeCell ref="G293:G301"/>
-    <mergeCell ref="E302:F302"/>
-    <mergeCell ref="A303:A311"/>
-    <mergeCell ref="G303:G311"/>
-    <mergeCell ref="E273:F273"/>
-    <mergeCell ref="A274:A281"/>
-    <mergeCell ref="G274:G281"/>
-    <mergeCell ref="E282:F282"/>
-    <mergeCell ref="A283:A291"/>
-    <mergeCell ref="G283:G291"/>
-    <mergeCell ref="E253:F253"/>
-    <mergeCell ref="A254:A262"/>
-    <mergeCell ref="G254:G262"/>
-    <mergeCell ref="E263:F263"/>
-    <mergeCell ref="A264:A272"/>
-    <mergeCell ref="G264:G272"/>
-    <mergeCell ref="E233:F233"/>
-    <mergeCell ref="A234:A242"/>
-    <mergeCell ref="G234:G242"/>
-    <mergeCell ref="E243:F243"/>
-    <mergeCell ref="A244:A252"/>
-    <mergeCell ref="G244:G252"/>
-    <mergeCell ref="E210:F210"/>
-    <mergeCell ref="A211:A220"/>
-    <mergeCell ref="G211:G220"/>
-    <mergeCell ref="E221:F221"/>
-    <mergeCell ref="A222:A232"/>
-    <mergeCell ref="G222:G232"/>
-    <mergeCell ref="E187:F187"/>
-    <mergeCell ref="A188:A196"/>
-    <mergeCell ref="G188:G196"/>
-    <mergeCell ref="E197:F197"/>
-    <mergeCell ref="A198:A209"/>
-    <mergeCell ref="G198:G209"/>
-    <mergeCell ref="E167:F167"/>
-    <mergeCell ref="A168:A176"/>
-    <mergeCell ref="G168:G176"/>
-    <mergeCell ref="E177:F177"/>
-    <mergeCell ref="A178:A186"/>
-    <mergeCell ref="G178:G186"/>
-    <mergeCell ref="E147:F147"/>
-    <mergeCell ref="A148:A156"/>
-    <mergeCell ref="G148:G156"/>
-    <mergeCell ref="E157:F157"/>
-    <mergeCell ref="A158:A166"/>
-    <mergeCell ref="G158:G166"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="A129:A137"/>
-    <mergeCell ref="G129:G137"/>
-    <mergeCell ref="E138:F138"/>
-    <mergeCell ref="A139:A146"/>
-    <mergeCell ref="G139:G146"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="A109:A117"/>
-    <mergeCell ref="G109:G117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="A119:A127"/>
-    <mergeCell ref="G119:G127"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="A89:A97"/>
-    <mergeCell ref="G89:G97"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="A99:A107"/>
-    <mergeCell ref="G99:G107"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:A74"/>
-    <mergeCell ref="G65:G74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="A76:A87"/>
-    <mergeCell ref="G76:G87"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="G55:G63"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A21:A32"/>
-    <mergeCell ref="G21:G32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="G34:G43"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="G11:G19"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="A45:A53"/>
-    <mergeCell ref="G45:G53"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A34:A43" r:id="rId1" display="Click here for the 1930 season football articles " xr:uid="{27C891E4-8C40-43BB-A88A-3796DCB1CA81}"/>

</xml_diff>